<commit_message>
[Feature]: calculate metrics on whole dataset.
</commit_message>
<xml_diff>
--- a/eval/classification_metrics_train.xlsx
+++ b/eval/classification_metrics_train.xlsx
@@ -471,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>18</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
@@ -490,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8125</v>
+        <v>0.8369704749679076</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.896551724137931</v>
+        <v>0.9112508735150244</v>
       </c>
       <c r="E4" t="n">
-        <v>130</v>
+        <v>652</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8125</v>
+        <v>0.8369704749679076</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8125</v>
+        <v>0.8369704749679076</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8125</v>
+        <v>0.8369704749679076</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8125</v>
+        <v>0.8369704749679076</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2708333333333333</v>
+        <v>0.2789901583226359</v>
       </c>
       <c r="C6" t="n">
         <v>0.3333333333333333</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2988505747126437</v>
+        <v>0.3037502911716748</v>
       </c>
       <c r="E6" t="n">
-        <v>160</v>
+        <v>779</v>
       </c>
     </row>
     <row r="7">
@@ -557,16 +557,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.66015625</v>
+        <v>0.7005195759680047</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8125</v>
+        <v>0.8369704749679076</v>
       </c>
       <c r="D7" t="n">
-        <v>0.728448275862069</v>
+        <v>0.7626900764207907</v>
       </c>
       <c r="E7" t="n">
-        <v>160</v>
+        <v>779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>